<commit_message>
add identifier column to spreadsheet
</commit_message>
<xml_diff>
--- a/manjanotas.xlsx
+++ b/manjanotas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>CNPJ</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Avenida República do Chile, 51</t>
+  </si>
+  <si>
+    <t>Identificador</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -548,60 +551,70 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started filling in page with Geb
</commit_message>
<xml_diff>
--- a/manjanotas.xlsx
+++ b/manjanotas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>CNPJ</t>
   </si>
@@ -34,9 +34,6 @@
     <t>62.100.755/0001-15</t>
   </si>
   <si>
-    <t>Rua Presidente Kennedy, 57</t>
-  </si>
-  <si>
     <t>Cidade</t>
   </si>
   <si>
@@ -70,17 +67,59 @@
     <t>78.865.726/0001-84</t>
   </si>
   <si>
-    <t>Avenida República do Chile, 51</t>
-  </si>
-  <si>
     <t>Identificador</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t>Complemento</t>
+  </si>
+  <si>
+    <t>Bairro</t>
+  </si>
+  <si>
+    <t>Telefone</t>
+  </si>
+  <si>
+    <t>Rua Presidente Kennedy</t>
+  </si>
+  <si>
+    <t>Casa 05</t>
+  </si>
+  <si>
+    <t>Cônego</t>
+  </si>
+  <si>
+    <t>(22) 2522-5120</t>
+  </si>
+  <si>
+    <t>Avenida República do Chile</t>
+  </si>
+  <si>
+    <t>Tijuca</t>
+  </si>
+  <si>
+    <t>(22) 2513-0056</t>
+  </si>
+  <si>
+    <t>Apto 212</t>
+  </si>
+  <si>
+    <t>(21) 2135-1448</t>
+  </si>
+  <si>
+    <t>Centro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +151,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +177,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -170,12 +217,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -195,6 +263,16 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -214,6 +292,16 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -543,27 +631,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
+    <row r="1" spans="1:11" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -572,13 +666,28 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -589,33 +698,60 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="J2">
+        <v>28621000</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>20031912</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -631,10 +767,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -642,12 +778,14 @@
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -656,27 +794,57 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>20510150</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactored invoice generation to use Manjerico data as the sender
</commit_message>
<xml_diff>
--- a/manjanotas.xlsx
+++ b/manjanotas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>CNPJ</t>
   </si>
@@ -55,9 +55,6 @@
     <t>06.828.467/0001-00</t>
   </si>
   <si>
-    <t>Rua Itacuruçá, 26</t>
-  </si>
-  <si>
     <t>Rio de Janeiro</t>
   </si>
   <si>
@@ -113,6 +110,15 @@
   </si>
   <si>
     <t>Centro</t>
+  </si>
+  <si>
+    <t>Rua Itacuruçá</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>manjerico@manjerico.com.br</t>
   </si>
 </sst>
 </file>
@@ -177,7 +183,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -237,13 +243,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="59"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="60">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -302,6 +310,7 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -654,7 +663,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -666,13 +675,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -681,10 +690,10 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -698,16 +707,16 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>57</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -719,7 +728,7 @@
         <v>28621000</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -727,22 +736,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3">
         <v>65</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3" t="s">
         <v>7</v>
@@ -751,7 +760,7 @@
         <v>20031912</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -767,10 +776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="K1" sqref="K1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -783,7 +792,7 @@
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -794,13 +803,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -809,13 +818,16 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -823,19 +835,19 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
@@ -844,10 +856,16 @@
         <v>20510150</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>